<commit_message>
Decreased charge current from 500mA to 100mA
R3 changed from 2K to 10K
</commit_message>
<xml_diff>
--- a/tinybot_BOM.xlsx
+++ b/tinybot_BOM.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikor\Documents\GitHub\tinybot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14940"/>
   </bookViews>
   <sheets>
     <sheet name="tinybot_BOM.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -102,9 +107,6 @@
     <t>R3</t>
   </si>
   <si>
-    <t>2 Kohm resistor</t>
-  </si>
-  <si>
     <t>RED</t>
   </si>
   <si>
@@ -246,12 +248,6 @@
     <t>MF1/4DC1000F</t>
   </si>
   <si>
-    <t>660-MF1/4DC2001F</t>
-  </si>
-  <si>
-    <t>MF1/4DC2001F</t>
-  </si>
-  <si>
     <t>Lots of 100 Robots (each)</t>
   </si>
   <si>
@@ -277,6 +273,15 @@
   </si>
   <si>
     <t>Ebay (http://goo.gl/HYa7EU)</t>
+  </si>
+  <si>
+    <t>10 Kohm resistor</t>
+  </si>
+  <si>
+    <t>660-MF1/4DC1002F</t>
+  </si>
+  <si>
+    <t>MF1/4DC1002F</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1251,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1257,41 +1262,41 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="8.83203125" style="2"/>
-    <col min="3" max="3" width="20.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="3"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="20.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.5" customWidth="1"/>
-    <col min="9" max="9" width="35.5" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" customWidth="1"/>
-    <col min="11" max="13" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="13" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K1" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L1" s="22"/>
       <c r="M1" s="23"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>1</v>
@@ -1309,33 +1314,33 @@
         <v>5</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>3</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G3" s="1">
         <v>0.95</v>
@@ -1345,10 +1350,10 @@
         <v>0.95</v>
       </c>
       <c r="I3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K3" s="18">
         <v>0.95</v>
@@ -1361,7 +1366,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1068</v>
       </c>
@@ -1372,13 +1377,13 @@
         <v>1068</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
         <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
       </c>
       <c r="G4" s="1">
         <v>1.79</v>
@@ -1388,10 +1393,10 @@
         <v>1.79</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K4" s="18">
         <v>1.6</v>
@@ -1404,24 +1409,24 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
       </c>
       <c r="G5" s="1">
         <v>1.4</v>
@@ -1431,10 +1436,10 @@
         <v>1.4</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K5" s="18">
         <v>0.62</v>
@@ -1447,24 +1452,24 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
       </c>
       <c r="G6" s="1">
         <v>1.32</v>
@@ -1477,7 +1482,7 @@
         <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K6" s="18">
         <v>0.78</v>
@@ -1490,9 +1495,9 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -1501,13 +1506,13 @@
         <v>9073</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1">
         <v>0.83</v>
@@ -1517,10 +1522,10 @@
         <v>1.66</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K7" s="18">
         <v>0.64</v>
@@ -1533,7 +1538,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1544,7 +1549,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -1563,7 +1568,7 @@
         <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K8" s="18">
         <v>0.42</v>
@@ -1576,7 +1581,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1587,7 +1592,7 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -1606,7 +1611,7 @@
         <v>9</v>
       </c>
       <c r="J9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K9" s="18">
         <v>0.14000000000000001</v>
@@ -1619,7 +1624,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1627,13 +1632,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
         <v>63</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>64</v>
       </c>
       <c r="F10" t="s">
         <v>18</v>
@@ -1649,7 +1654,7 @@
         <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K10" s="18">
         <v>0.1</v>
@@ -1662,7 +1667,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1670,13 +1675,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
         <v>21</v>
@@ -1692,7 +1697,7 @@
         <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K11" s="18">
         <v>0.09</v>
@@ -1705,24 +1710,24 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
         <v>59</v>
       </c>
-      <c r="E12" t="s">
-        <v>60</v>
-      </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="1">
         <v>0.1</v>
@@ -1735,7 +1740,7 @@
         <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K12" s="18">
         <v>0.08</v>
@@ -1748,7 +1753,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1756,13 +1761,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
         <v>56</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>57</v>
-      </c>
-      <c r="E13" t="s">
-        <v>58</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -1778,7 +1783,7 @@
         <v>9</v>
       </c>
       <c r="J13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K13" s="18">
         <v>0.04</v>
@@ -1791,24 +1796,24 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
         <v>68</v>
       </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" t="s">
-        <v>69</v>
-      </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="1">
         <v>0.08</v>
@@ -1821,7 +1826,7 @@
         <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K14" s="18">
         <v>0.06</v>
@@ -1834,7 +1839,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -1842,13 +1847,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
         <v>23</v>
@@ -1864,7 +1869,7 @@
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K15" s="18">
         <v>0.04</v>
@@ -1877,7 +1882,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -1885,13 +1890,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
         <v>71</v>
-      </c>
-      <c r="D16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" t="s">
-        <v>72</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
@@ -1907,7 +1912,7 @@
         <v>19</v>
       </c>
       <c r="J16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K16" s="18">
         <v>0.04</v>
@@ -1920,7 +1925,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
@@ -1928,16 +1933,16 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="G17" s="1">
         <v>0.05</v>
@@ -1950,7 +1955,7 @@
         <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K17" s="18">
         <v>0.04</v>
@@ -1963,9 +1968,9 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="11" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="18" spans="1:13" s="11" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="7"/>
@@ -1986,12 +1991,12 @@
         <v>6.42</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>